<commit_message>
partner brand type finally addded in both executive side and admin side
</commit_message>
<xml_diff>
--- a/public/templates/store-import-template.xlsx
+++ b/public/templates/store-import-template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\visha\Desktop\New folder (4)\Zopper\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC60A237-8046-4834-B121-D00215DA4BEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFB91F0D-5610-4860-901E-C7D50889EAE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -513,7 +513,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="99" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>